<commit_message>
define template from scanner
</commit_message>
<xml_diff>
--- a/OEE_OMR_border.xlsx
+++ b/OEE_OMR_border.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Halima Mohmed\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismail.mohammed\TempScripts\openCV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292EF34C-5B7F-452C-8ED3-A7971CDD8150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F8D3C3-9962-47AF-BD41-4AF41FD0583F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4785" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{190001B4-36A3-4661-BC69-593BA84E0A7A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{190001B4-36A3-4661-BC69-593BA84E0A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="FULLSHEET" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="84">
   <si>
     <t></t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t></t>
+  </si>
+  <si>
+    <t>LEFT INDENT FILLED SPOT ON TEMPLATE THAT REPRESENT NUMBERS!</t>
   </si>
 </sst>
 </file>
@@ -962,7 +965,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1329,6 +1332,30 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1347,6 +1374,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1365,39 +1416,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1405,7 +1423,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1723,8 +1741,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="457200" y="2085975"/>
-          <a:ext cx="4629150" cy="845185"/>
+          <a:off x="479425" y="2085975"/>
+          <a:ext cx="4829175" cy="845185"/>
           <a:chOff x="0" y="-121749"/>
           <a:chExt cx="5067306" cy="845401"/>
         </a:xfrm>
@@ -2361,19 +2379,19 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.4" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="26" width="3.28515625" customWidth="1"/>
-    <col min="27" max="27" width="4.7109375" style="32" customWidth="1"/>
-    <col min="28" max="34" width="3.28515625" customWidth="1"/>
-    <col min="35" max="35" width="3.28515625" style="32" customWidth="1"/>
-    <col min="36" max="36" width="4.7109375" customWidth="1"/>
-    <col min="37" max="43" width="3.28515625" customWidth="1"/>
-    <col min="44" max="44" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
+    <col min="2" max="26" width="3.26953125" customWidth="1"/>
+    <col min="27" max="27" width="4.7265625" style="32" customWidth="1"/>
+    <col min="28" max="34" width="3.26953125" customWidth="1"/>
+    <col min="35" max="35" width="3.26953125" style="32" customWidth="1"/>
+    <col min="36" max="36" width="4.7265625" customWidth="1"/>
+    <col min="37" max="43" width="3.26953125" customWidth="1"/>
+    <col min="44" max="44" width="3.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="82"/>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -2419,7 +2437,7 @@
       <c r="AQ1" s="83"/>
       <c r="AR1" s="85"/>
     </row>
-    <row r="2" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="86"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2433,20 +2451,20 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="152" t="s">
+      <c r="N2" s="145" t="s">
         <v>79</v>
       </c>
-      <c r="O2" s="152"/>
-      <c r="P2" s="152"/>
-      <c r="Q2" s="152"/>
-      <c r="R2" s="152"/>
-      <c r="S2" s="152"/>
-      <c r="T2" s="152"/>
-      <c r="U2" s="152"/>
-      <c r="V2" s="152"/>
-      <c r="W2" s="152"/>
-      <c r="X2" s="152"/>
-      <c r="Y2" s="152"/>
+      <c r="O2" s="145"/>
+      <c r="P2" s="145"/>
+      <c r="Q2" s="145"/>
+      <c r="R2" s="145"/>
+      <c r="S2" s="145"/>
+      <c r="T2" s="145"/>
+      <c r="U2" s="145"/>
+      <c r="V2" s="145"/>
+      <c r="W2" s="145"/>
+      <c r="X2" s="145"/>
+      <c r="Y2" s="145"/>
       <c r="Z2" s="87"/>
       <c r="AA2" s="34"/>
       <c r="AB2" s="1"/>
@@ -2467,7 +2485,7 @@
       <c r="AQ2" s="1"/>
       <c r="AR2" s="88"/>
     </row>
-    <row r="3" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="86"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2481,18 +2499,18 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="152"/>
-      <c r="O3" s="152"/>
-      <c r="P3" s="152"/>
-      <c r="Q3" s="152"/>
-      <c r="R3" s="152"/>
-      <c r="S3" s="152"/>
-      <c r="T3" s="152"/>
-      <c r="U3" s="152"/>
-      <c r="V3" s="152"/>
-      <c r="W3" s="152"/>
-      <c r="X3" s="152"/>
-      <c r="Y3" s="152"/>
+      <c r="N3" s="145"/>
+      <c r="O3" s="145"/>
+      <c r="P3" s="145"/>
+      <c r="Q3" s="145"/>
+      <c r="R3" s="145"/>
+      <c r="S3" s="145"/>
+      <c r="T3" s="145"/>
+      <c r="U3" s="145"/>
+      <c r="V3" s="145"/>
+      <c r="W3" s="145"/>
+      <c r="X3" s="145"/>
+      <c r="Y3" s="145"/>
       <c r="Z3" s="87"/>
       <c r="AA3" s="34"/>
       <c r="AB3" s="1"/>
@@ -2513,7 +2531,7 @@
       <c r="AQ3" s="1"/>
       <c r="AR3" s="88"/>
     </row>
-    <row r="4" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="86"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2527,20 +2545,20 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="153" t="s">
+      <c r="N4" s="146" t="s">
         <v>80</v>
       </c>
-      <c r="O4" s="153"/>
-      <c r="P4" s="153"/>
-      <c r="Q4" s="153"/>
-      <c r="R4" s="153"/>
-      <c r="S4" s="153"/>
-      <c r="T4" s="153"/>
-      <c r="U4" s="153"/>
-      <c r="V4" s="153"/>
-      <c r="W4" s="153"/>
-      <c r="X4" s="153"/>
-      <c r="Y4" s="153"/>
+      <c r="O4" s="146"/>
+      <c r="P4" s="146"/>
+      <c r="Q4" s="146"/>
+      <c r="R4" s="146"/>
+      <c r="S4" s="146"/>
+      <c r="T4" s="146"/>
+      <c r="U4" s="146"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="146"/>
       <c r="Z4" s="89"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="1"/>
@@ -2561,7 +2579,7 @@
       <c r="AQ4" s="1"/>
       <c r="AR4" s="88"/>
     </row>
-    <row r="5" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="86"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2575,18 +2593,18 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="153"/>
-      <c r="O5" s="153"/>
-      <c r="P5" s="153"/>
-      <c r="Q5" s="153"/>
-      <c r="R5" s="153"/>
-      <c r="S5" s="153"/>
-      <c r="T5" s="153"/>
-      <c r="U5" s="153"/>
-      <c r="V5" s="153"/>
-      <c r="W5" s="153"/>
-      <c r="X5" s="153"/>
-      <c r="Y5" s="153"/>
+      <c r="N5" s="146"/>
+      <c r="O5" s="146"/>
+      <c r="P5" s="146"/>
+      <c r="Q5" s="146"/>
+      <c r="R5" s="146"/>
+      <c r="S5" s="146"/>
+      <c r="T5" s="146"/>
+      <c r="U5" s="146"/>
+      <c r="V5" s="146"/>
+      <c r="W5" s="146"/>
+      <c r="X5" s="146"/>
+      <c r="Y5" s="146"/>
       <c r="Z5" s="89"/>
       <c r="AA5" s="34"/>
       <c r="AB5" s="1"/>
@@ -2607,7 +2625,7 @@
       <c r="AQ5" s="1"/>
       <c r="AR5" s="88"/>
     </row>
-    <row r="6" spans="1:44" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="86"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2621,18 +2639,18 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="153"/>
-      <c r="O6" s="153"/>
-      <c r="P6" s="153"/>
-      <c r="Q6" s="153"/>
-      <c r="R6" s="153"/>
-      <c r="S6" s="153"/>
-      <c r="T6" s="153"/>
-      <c r="U6" s="153"/>
-      <c r="V6" s="153"/>
-      <c r="W6" s="153"/>
-      <c r="X6" s="153"/>
-      <c r="Y6" s="153"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="146"/>
+      <c r="P6" s="146"/>
+      <c r="Q6" s="146"/>
+      <c r="R6" s="146"/>
+      <c r="S6" s="146"/>
+      <c r="T6" s="146"/>
+      <c r="U6" s="146"/>
+      <c r="V6" s="146"/>
+      <c r="W6" s="146"/>
+      <c r="X6" s="146"/>
+      <c r="Y6" s="146"/>
       <c r="Z6" s="89"/>
       <c r="AA6" s="105" t="s">
         <v>33</v>
@@ -2661,7 +2679,7 @@
       <c r="AQ6" s="112"/>
       <c r="AR6" s="88"/>
     </row>
-    <row r="7" spans="1:44" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="86"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2675,18 +2693,18 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="153"/>
-      <c r="O7" s="153"/>
-      <c r="P7" s="153"/>
-      <c r="Q7" s="153"/>
-      <c r="R7" s="153"/>
-      <c r="S7" s="153"/>
-      <c r="T7" s="153"/>
-      <c r="U7" s="153"/>
-      <c r="V7" s="153"/>
-      <c r="W7" s="153"/>
-      <c r="X7" s="153"/>
-      <c r="Y7" s="153"/>
+      <c r="N7" s="146"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="146"/>
+      <c r="R7" s="146"/>
+      <c r="S7" s="146"/>
+      <c r="T7" s="146"/>
+      <c r="U7" s="146"/>
+      <c r="V7" s="146"/>
+      <c r="W7" s="146"/>
+      <c r="X7" s="146"/>
+      <c r="Y7" s="146"/>
       <c r="Z7" s="89"/>
       <c r="AA7" s="113" t="s">
         <v>8</v>
@@ -2719,7 +2737,7 @@
       <c r="AQ7" s="114"/>
       <c r="AR7" s="88"/>
     </row>
-    <row r="8" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="86"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2733,20 +2751,20 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="154" t="s">
+      <c r="N8" s="147" t="s">
         <v>78</v>
       </c>
-      <c r="O8" s="154"/>
-      <c r="P8" s="154"/>
-      <c r="Q8" s="154"/>
-      <c r="R8" s="154"/>
-      <c r="S8" s="154"/>
-      <c r="T8" s="154"/>
-      <c r="U8" s="154"/>
-      <c r="V8" s="154"/>
-      <c r="W8" s="154"/>
-      <c r="X8" s="154"/>
-      <c r="Y8" s="154"/>
+      <c r="O8" s="147"/>
+      <c r="P8" s="147"/>
+      <c r="Q8" s="147"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="147"/>
+      <c r="T8" s="147"/>
+      <c r="U8" s="147"/>
+      <c r="V8" s="147"/>
+      <c r="W8" s="147"/>
+      <c r="X8" s="147"/>
+      <c r="Y8" s="147"/>
       <c r="Z8" s="90"/>
       <c r="AA8" s="115" t="s">
         <v>9</v>
@@ -2799,7 +2817,7 @@
       </c>
       <c r="AR8" s="88"/>
     </row>
-    <row r="9" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="86"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2877,7 +2895,7 @@
       </c>
       <c r="AR9" s="88"/>
     </row>
-    <row r="10" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="86"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2955,7 +2973,7 @@
       </c>
       <c r="AR10" s="88"/>
     </row>
-    <row r="11" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="86"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -3033,7 +3051,7 @@
       </c>
       <c r="AR11" s="88"/>
     </row>
-    <row r="12" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="86"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -3111,7 +3129,7 @@
       </c>
       <c r="AR12" s="88"/>
     </row>
-    <row r="13" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="86"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -3189,7 +3207,7 @@
       </c>
       <c r="AR13" s="88"/>
     </row>
-    <row r="14" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="86"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -3267,7 +3285,7 @@
       </c>
       <c r="AR14" s="88"/>
     </row>
-    <row r="15" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="86"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -3345,7 +3363,7 @@
       </c>
       <c r="AR15" s="88"/>
     </row>
-    <row r="16" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="86"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -3423,7 +3441,7 @@
       </c>
       <c r="AR16" s="88"/>
     </row>
-    <row r="17" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="86"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -3501,7 +3519,7 @@
       </c>
       <c r="AR17" s="88"/>
     </row>
-    <row r="18" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="86"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -3547,48 +3565,48 @@
       <c r="AQ18" s="120"/>
       <c r="AR18" s="88"/>
     </row>
-    <row r="19" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="86"/>
-      <c r="B19" s="140" t="s">
+      <c r="B19" s="148" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="142"/>
-      <c r="D19" s="140" t="s">
+      <c r="C19" s="150"/>
+      <c r="D19" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="142"/>
+      <c r="E19" s="150"/>
       <c r="F19" s="53" t="s">
         <v>49</v>
       </c>
       <c r="G19" s="52"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="158" t="s">
+      <c r="J19" s="157" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="159"/>
-      <c r="L19" s="159"/>
-      <c r="M19" s="159"/>
-      <c r="N19" s="159"/>
-      <c r="O19" s="159"/>
-      <c r="P19" s="159"/>
-      <c r="Q19" s="159"/>
-      <c r="R19" s="159"/>
-      <c r="S19" s="159"/>
-      <c r="T19" s="159"/>
-      <c r="U19" s="159"/>
-      <c r="V19" s="159"/>
-      <c r="W19" s="159"/>
-      <c r="X19" s="159"/>
-      <c r="Y19" s="160"/>
+      <c r="K19" s="158"/>
+      <c r="L19" s="158"/>
+      <c r="M19" s="158"/>
+      <c r="N19" s="158"/>
+      <c r="O19" s="158"/>
+      <c r="P19" s="158"/>
+      <c r="Q19" s="158"/>
+      <c r="R19" s="158"/>
+      <c r="S19" s="158"/>
+      <c r="T19" s="158"/>
+      <c r="U19" s="158"/>
+      <c r="V19" s="158"/>
+      <c r="W19" s="158"/>
+      <c r="X19" s="158"/>
+      <c r="Y19" s="159"/>
       <c r="Z19" s="25"/>
-      <c r="AA19" s="161" t="s">
+      <c r="AA19" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="AB19" s="162"/>
-      <c r="AC19" s="162"/>
-      <c r="AD19" s="162"/>
-      <c r="AE19" s="162"/>
+      <c r="AB19" s="161"/>
+      <c r="AC19" s="161"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
       <c r="AF19" s="73" t="s">
         <v>17</v>
       </c>
@@ -3609,7 +3627,7 @@
       <c r="AQ19" s="121"/>
       <c r="AR19" s="88"/>
     </row>
-    <row r="20" spans="1:44" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A20" s="86"/>
       <c r="B20" s="130" t="s">
         <v>14</v>
@@ -3664,20 +3682,20 @@
         <v>0</v>
       </c>
       <c r="Z20" s="25"/>
-      <c r="AA20" s="151" t="s">
+      <c r="AA20" s="167" t="s">
         <v>8</v>
       </c>
-      <c r="AB20" s="149"/>
-      <c r="AC20" s="149" t="s">
+      <c r="AB20" s="165"/>
+      <c r="AC20" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="AD20" s="149"/>
-      <c r="AE20" s="150"/>
-      <c r="AF20" s="146" t="s">
+      <c r="AD20" s="165"/>
+      <c r="AE20" s="166"/>
+      <c r="AF20" s="162" t="s">
         <v>32</v>
       </c>
-      <c r="AG20" s="147"/>
-      <c r="AH20" s="148"/>
+      <c r="AG20" s="163"/>
+      <c r="AH20" s="164"/>
       <c r="AI20" s="34"/>
       <c r="AJ20" s="101" t="s">
         <v>8</v>
@@ -3695,7 +3713,7 @@
       <c r="AQ20" s="114"/>
       <c r="AR20" s="88"/>
     </row>
-    <row r="21" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="86"/>
       <c r="B21" s="68" t="s">
         <v>15</v>
@@ -3801,7 +3819,7 @@
       </c>
       <c r="AR21" s="88"/>
     </row>
-    <row r="22" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="86"/>
       <c r="B22" s="68" t="s">
         <v>16</v>
@@ -3907,7 +3925,7 @@
       </c>
       <c r="AR22" s="88"/>
     </row>
-    <row r="23" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="86"/>
       <c r="B23" s="68" t="s">
         <v>17</v>
@@ -4013,7 +4031,7 @@
       </c>
       <c r="AR23" s="88"/>
     </row>
-    <row r="24" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="86"/>
       <c r="B24" s="68"/>
       <c r="C24" s="14" t="s">
@@ -4101,7 +4119,7 @@
       </c>
       <c r="AR24" s="88"/>
     </row>
-    <row r="25" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="86"/>
       <c r="B25" s="68"/>
       <c r="C25" s="14" t="s">
@@ -4123,18 +4141,18 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="143" t="s">
+      <c r="P25" s="151" t="s">
         <v>30</v>
       </c>
-      <c r="Q25" s="144"/>
-      <c r="R25" s="144"/>
-      <c r="S25" s="144"/>
-      <c r="T25" s="144"/>
-      <c r="U25" s="144"/>
-      <c r="V25" s="144"/>
-      <c r="W25" s="144"/>
-      <c r="X25" s="144"/>
-      <c r="Y25" s="145"/>
+      <c r="Q25" s="152"/>
+      <c r="R25" s="152"/>
+      <c r="S25" s="152"/>
+      <c r="T25" s="152"/>
+      <c r="U25" s="152"/>
+      <c r="V25" s="152"/>
+      <c r="W25" s="152"/>
+      <c r="X25" s="152"/>
+      <c r="Y25" s="153"/>
       <c r="Z25" s="12"/>
       <c r="AA25" s="115" t="s">
         <v>3</v>
@@ -4187,7 +4205,7 @@
       </c>
       <c r="AR25" s="88"/>
     </row>
-    <row r="26" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="86"/>
       <c r="B26" s="68"/>
       <c r="C26" s="14" t="s">
@@ -4209,20 +4227,20 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="143" t="s">
+      <c r="P26" s="151" t="s">
         <v>74</v>
       </c>
-      <c r="Q26" s="144"/>
-      <c r="R26" s="144"/>
-      <c r="S26" s="144"/>
-      <c r="T26" s="145"/>
-      <c r="U26" s="143" t="s">
+      <c r="Q26" s="152"/>
+      <c r="R26" s="152"/>
+      <c r="S26" s="152"/>
+      <c r="T26" s="153"/>
+      <c r="U26" s="151" t="s">
         <v>75</v>
       </c>
-      <c r="V26" s="144"/>
-      <c r="W26" s="144"/>
-      <c r="X26" s="144"/>
-      <c r="Y26" s="145"/>
+      <c r="V26" s="152"/>
+      <c r="W26" s="152"/>
+      <c r="X26" s="152"/>
+      <c r="Y26" s="153"/>
       <c r="Z26" s="13"/>
       <c r="AA26" s="115" t="s">
         <v>5</v>
@@ -4275,7 +4293,7 @@
       </c>
       <c r="AR26" s="88"/>
     </row>
-    <row r="27" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="86"/>
       <c r="B27" s="68"/>
       <c r="C27" s="14" t="s">
@@ -4367,7 +4385,7 @@
       </c>
       <c r="AR27" s="88"/>
     </row>
-    <row r="28" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="86"/>
       <c r="B28" s="68"/>
       <c r="C28" s="14" t="s">
@@ -4382,13 +4400,13 @@
       <c r="F28" s="1"/>
       <c r="G28" s="48"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="140" t="s">
+      <c r="I28" s="148" t="s">
         <v>62</v>
       </c>
-      <c r="J28" s="141"/>
-      <c r="K28" s="141"/>
-      <c r="L28" s="141"/>
-      <c r="M28" s="142"/>
+      <c r="J28" s="149"/>
+      <c r="K28" s="149"/>
+      <c r="L28" s="149"/>
+      <c r="M28" s="150"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="77" t="s">
@@ -4461,7 +4479,7 @@
       </c>
       <c r="AR28" s="88"/>
     </row>
-    <row r="29" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="86"/>
       <c r="B29" s="69"/>
       <c r="C29" s="14" t="s">
@@ -4559,7 +4577,7 @@
       </c>
       <c r="AR29" s="88"/>
     </row>
-    <row r="30" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="86"/>
       <c r="B30" s="59"/>
       <c r="C30" s="1"/>
@@ -4655,7 +4673,7 @@
       </c>
       <c r="AR30" s="88"/>
     </row>
-    <row r="31" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="86"/>
       <c r="B31" s="60"/>
       <c r="C31" s="61"/>
@@ -4709,7 +4727,7 @@
       <c r="AQ31" s="120"/>
       <c r="AR31" s="88"/>
     </row>
-    <row r="32" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="86"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4763,7 +4781,7 @@
       <c r="AQ32" s="121"/>
       <c r="AR32" s="88"/>
     </row>
-    <row r="33" spans="1:44" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A33" s="86"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -4821,40 +4839,40 @@
       <c r="AQ33" s="114"/>
       <c r="AR33" s="88"/>
     </row>
-    <row r="34" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="86"/>
       <c r="B34" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="140" t="s">
+      <c r="C34" s="148" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="141"/>
-      <c r="E34" s="141"/>
-      <c r="F34" s="141"/>
-      <c r="G34" s="141"/>
-      <c r="H34" s="142"/>
-      <c r="I34" s="140" t="s">
+      <c r="D34" s="149"/>
+      <c r="E34" s="149"/>
+      <c r="F34" s="149"/>
+      <c r="G34" s="149"/>
+      <c r="H34" s="150"/>
+      <c r="I34" s="148" t="s">
         <v>81</v>
       </c>
-      <c r="J34" s="141"/>
-      <c r="K34" s="141"/>
-      <c r="L34" s="141"/>
-      <c r="M34" s="141"/>
-      <c r="N34" s="141"/>
-      <c r="O34" s="141"/>
-      <c r="P34" s="141"/>
-      <c r="Q34" s="141"/>
-      <c r="R34" s="142"/>
-      <c r="S34" s="155" t="s">
+      <c r="J34" s="149"/>
+      <c r="K34" s="149"/>
+      <c r="L34" s="149"/>
+      <c r="M34" s="149"/>
+      <c r="N34" s="149"/>
+      <c r="O34" s="149"/>
+      <c r="P34" s="149"/>
+      <c r="Q34" s="149"/>
+      <c r="R34" s="150"/>
+      <c r="S34" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="T34" s="156"/>
-      <c r="U34" s="156"/>
-      <c r="V34" s="156"/>
-      <c r="W34" s="156"/>
-      <c r="X34" s="156"/>
-      <c r="Y34" s="157"/>
+      <c r="T34" s="155"/>
+      <c r="U34" s="155"/>
+      <c r="V34" s="155"/>
+      <c r="W34" s="155"/>
+      <c r="X34" s="155"/>
+      <c r="Y34" s="156"/>
       <c r="Z34" s="40"/>
       <c r="AA34" s="115" t="s">
         <v>9</v>
@@ -4907,7 +4925,7 @@
       </c>
       <c r="AR34" s="88"/>
     </row>
-    <row r="35" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="86"/>
       <c r="B35" s="72">
         <v>14</v>
@@ -5033,7 +5051,7 @@
       </c>
       <c r="AR35" s="88"/>
     </row>
-    <row r="36" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="86"/>
       <c r="B36" s="80">
         <f>B35+1</f>
@@ -5160,7 +5178,7 @@
       </c>
       <c r="AR36" s="88"/>
     </row>
-    <row r="37" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="86"/>
       <c r="B37" s="80">
         <f>B36+1</f>
@@ -5287,7 +5305,7 @@
       </c>
       <c r="AR37" s="88"/>
     </row>
-    <row r="38" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="86"/>
       <c r="B38" s="80">
         <f>B37+1</f>
@@ -5414,7 +5432,7 @@
       </c>
       <c r="AR38" s="88"/>
     </row>
-    <row r="39" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="86"/>
       <c r="B39" s="72">
         <f>B38+1</f>
@@ -5541,7 +5559,7 @@
       </c>
       <c r="AR39" s="88"/>
     </row>
-    <row r="40" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="86"/>
       <c r="B40" s="80">
         <f t="shared" ref="B40:B42" si="0">B39+1</f>
@@ -5668,7 +5686,7 @@
       </c>
       <c r="AR40" s="88"/>
     </row>
-    <row r="41" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="86"/>
       <c r="B41" s="80">
         <f t="shared" si="0"/>
@@ -5795,7 +5813,7 @@
       </c>
       <c r="AR41" s="88"/>
     </row>
-    <row r="42" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="86"/>
       <c r="B42" s="80">
         <f t="shared" si="0"/>
@@ -5922,7 +5940,7 @@
       </c>
       <c r="AR42" s="88"/>
     </row>
-    <row r="43" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="86"/>
       <c r="B43" s="72">
         <f>B42+1</f>
@@ -6049,7 +6067,7 @@
       </c>
       <c r="AR43" s="88"/>
     </row>
-    <row r="44" spans="1:44" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A44" s="86"/>
       <c r="B44" s="80">
         <f t="shared" ref="B44" si="1">B43+1</f>
@@ -6144,7 +6162,7 @@
       <c r="AQ44" s="1"/>
       <c r="AR44" s="88"/>
     </row>
-    <row r="45" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="92"/>
       <c r="B45" s="93"/>
       <c r="C45" s="93"/>
@@ -6192,9 +6210,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="J19:Y19"/>
     <mergeCell ref="AA19:AE19"/>
     <mergeCell ref="AF20:AH20"/>
     <mergeCell ref="AC20:AE20"/>
@@ -6209,25 +6224,34 @@
     <mergeCell ref="I28:M28"/>
     <mergeCell ref="S34:Y34"/>
     <mergeCell ref="I34:R34"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="J19:Y19"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="98" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="94" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2494B356-85DC-4609-A2FF-95F28311FBEE}">
-  <dimension ref="A1"/>
+  <dimension ref="B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6240,23 +6264,23 @@
   </sheetPr>
   <dimension ref="A1:AR45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH17" sqref="AH17"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK14" sqref="AK14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.4" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="26" width="3.28515625" customWidth="1"/>
-    <col min="27" max="27" width="4.7109375" style="32" customWidth="1"/>
-    <col min="28" max="34" width="3.28515625" customWidth="1"/>
-    <col min="35" max="35" width="3.28515625" style="32" customWidth="1"/>
-    <col min="36" max="36" width="4.7109375" customWidth="1"/>
-    <col min="37" max="43" width="3.28515625" customWidth="1"/>
-    <col min="44" max="44" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
+    <col min="2" max="26" width="3.26953125" customWidth="1"/>
+    <col min="27" max="27" width="4.7265625" style="32" customWidth="1"/>
+    <col min="28" max="34" width="3.26953125" customWidth="1"/>
+    <col min="35" max="35" width="3.26953125" style="32" customWidth="1"/>
+    <col min="36" max="36" width="4.7265625" customWidth="1"/>
+    <col min="37" max="43" width="3.26953125" customWidth="1"/>
+    <col min="44" max="44" width="3.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="82"/>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -6302,7 +6326,7 @@
       <c r="AQ1" s="83"/>
       <c r="AR1" s="85"/>
     </row>
-    <row r="2" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="86"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -6316,18 +6340,18 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="152"/>
-      <c r="O2" s="152"/>
-      <c r="P2" s="152"/>
-      <c r="Q2" s="152"/>
-      <c r="R2" s="152"/>
-      <c r="S2" s="152"/>
-      <c r="T2" s="152"/>
-      <c r="U2" s="152"/>
-      <c r="V2" s="152"/>
-      <c r="W2" s="152"/>
-      <c r="X2" s="152"/>
-      <c r="Y2" s="152"/>
+      <c r="N2" s="145"/>
+      <c r="O2" s="145"/>
+      <c r="P2" s="145"/>
+      <c r="Q2" s="145"/>
+      <c r="R2" s="145"/>
+      <c r="S2" s="145"/>
+      <c r="T2" s="145"/>
+      <c r="U2" s="145"/>
+      <c r="V2" s="145"/>
+      <c r="W2" s="145"/>
+      <c r="X2" s="145"/>
+      <c r="Y2" s="145"/>
       <c r="Z2" s="87"/>
       <c r="AA2" s="34"/>
       <c r="AB2" s="1"/>
@@ -6348,7 +6372,7 @@
       <c r="AQ2" s="1"/>
       <c r="AR2" s="88"/>
     </row>
-    <row r="3" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="86"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -6362,18 +6386,18 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="152"/>
-      <c r="O3" s="152"/>
-      <c r="P3" s="152"/>
-      <c r="Q3" s="152"/>
-      <c r="R3" s="152"/>
-      <c r="S3" s="152"/>
-      <c r="T3" s="152"/>
-      <c r="U3" s="152"/>
-      <c r="V3" s="152"/>
-      <c r="W3" s="152"/>
-      <c r="X3" s="152"/>
-      <c r="Y3" s="152"/>
+      <c r="N3" s="145"/>
+      <c r="O3" s="145"/>
+      <c r="P3" s="145"/>
+      <c r="Q3" s="145"/>
+      <c r="R3" s="145"/>
+      <c r="S3" s="145"/>
+      <c r="T3" s="145"/>
+      <c r="U3" s="145"/>
+      <c r="V3" s="145"/>
+      <c r="W3" s="145"/>
+      <c r="X3" s="145"/>
+      <c r="Y3" s="145"/>
       <c r="Z3" s="87"/>
       <c r="AA3" s="34"/>
       <c r="AB3" s="1"/>
@@ -6394,7 +6418,7 @@
       <c r="AQ3" s="1"/>
       <c r="AR3" s="88"/>
     </row>
-    <row r="4" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="86"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -6408,18 +6432,18 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="153"/>
-      <c r="O4" s="153"/>
-      <c r="P4" s="153"/>
-      <c r="Q4" s="153"/>
-      <c r="R4" s="153"/>
-      <c r="S4" s="153"/>
-      <c r="T4" s="153"/>
-      <c r="U4" s="153"/>
-      <c r="V4" s="153"/>
-      <c r="W4" s="153"/>
-      <c r="X4" s="153"/>
-      <c r="Y4" s="153"/>
+      <c r="N4" s="146"/>
+      <c r="O4" s="146"/>
+      <c r="P4" s="146"/>
+      <c r="Q4" s="146"/>
+      <c r="R4" s="146"/>
+      <c r="S4" s="146"/>
+      <c r="T4" s="146"/>
+      <c r="U4" s="146"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="146"/>
       <c r="Z4" s="89"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="1"/>
@@ -6440,7 +6464,7 @@
       <c r="AQ4" s="1"/>
       <c r="AR4" s="88"/>
     </row>
-    <row r="5" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="86"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -6454,18 +6478,18 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="153"/>
-      <c r="O5" s="153"/>
-      <c r="P5" s="153"/>
-      <c r="Q5" s="153"/>
-      <c r="R5" s="153"/>
-      <c r="S5" s="153"/>
-      <c r="T5" s="153"/>
-      <c r="U5" s="153"/>
-      <c r="V5" s="153"/>
-      <c r="W5" s="153"/>
-      <c r="X5" s="153"/>
-      <c r="Y5" s="153"/>
+      <c r="N5" s="146"/>
+      <c r="O5" s="146"/>
+      <c r="P5" s="146"/>
+      <c r="Q5" s="146"/>
+      <c r="R5" s="146"/>
+      <c r="S5" s="146"/>
+      <c r="T5" s="146"/>
+      <c r="U5" s="146"/>
+      <c r="V5" s="146"/>
+      <c r="W5" s="146"/>
+      <c r="X5" s="146"/>
+      <c r="Y5" s="146"/>
       <c r="Z5" s="89"/>
       <c r="AA5" s="34"/>
       <c r="AB5" s="1"/>
@@ -6486,7 +6510,7 @@
       <c r="AQ5" s="1"/>
       <c r="AR5" s="88"/>
     </row>
-    <row r="6" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="86"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -6500,18 +6524,18 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="153"/>
-      <c r="O6" s="153"/>
-      <c r="P6" s="153"/>
-      <c r="Q6" s="153"/>
-      <c r="R6" s="153"/>
-      <c r="S6" s="153"/>
-      <c r="T6" s="153"/>
-      <c r="U6" s="153"/>
-      <c r="V6" s="153"/>
-      <c r="W6" s="153"/>
-      <c r="X6" s="153"/>
-      <c r="Y6" s="153"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="146"/>
+      <c r="P6" s="146"/>
+      <c r="Q6" s="146"/>
+      <c r="R6" s="146"/>
+      <c r="S6" s="146"/>
+      <c r="T6" s="146"/>
+      <c r="U6" s="146"/>
+      <c r="V6" s="146"/>
+      <c r="W6" s="146"/>
+      <c r="X6" s="146"/>
+      <c r="Y6" s="146"/>
       <c r="Z6" s="89"/>
       <c r="AA6" s="132"/>
       <c r="AB6" s="132"/>
@@ -6532,7 +6556,7 @@
       <c r="AQ6" s="74"/>
       <c r="AR6" s="88"/>
     </row>
-    <row r="7" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="86"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -6546,18 +6570,18 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="153"/>
-      <c r="O7" s="153"/>
-      <c r="P7" s="153"/>
-      <c r="Q7" s="153"/>
-      <c r="R7" s="153"/>
-      <c r="S7" s="153"/>
-      <c r="T7" s="153"/>
-      <c r="U7" s="153"/>
-      <c r="V7" s="153"/>
-      <c r="W7" s="153"/>
-      <c r="X7" s="153"/>
-      <c r="Y7" s="153"/>
+      <c r="N7" s="146"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="146"/>
+      <c r="R7" s="146"/>
+      <c r="S7" s="146"/>
+      <c r="T7" s="146"/>
+      <c r="U7" s="146"/>
+      <c r="V7" s="146"/>
+      <c r="W7" s="146"/>
+      <c r="X7" s="146"/>
+      <c r="Y7" s="146"/>
       <c r="Z7" s="89"/>
       <c r="AA7" s="134"/>
       <c r="AB7" s="134"/>
@@ -6578,7 +6602,7 @@
       <c r="AQ7" s="135"/>
       <c r="AR7" s="88"/>
     </row>
-    <row r="8" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="86"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6592,39 +6616,39 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="154"/>
-      <c r="O8" s="154"/>
-      <c r="P8" s="154"/>
-      <c r="Q8" s="154"/>
-      <c r="R8" s="154"/>
-      <c r="S8" s="154"/>
-      <c r="T8" s="154"/>
-      <c r="U8" s="154"/>
-      <c r="V8" s="154"/>
-      <c r="W8" s="154"/>
-      <c r="X8" s="154"/>
-      <c r="Y8" s="154"/>
+      <c r="N8" s="147"/>
+      <c r="O8" s="147"/>
+      <c r="P8" s="147"/>
+      <c r="Q8" s="147"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="147"/>
+      <c r="T8" s="147"/>
+      <c r="U8" s="147"/>
+      <c r="V8" s="147"/>
+      <c r="W8" s="147"/>
+      <c r="X8" s="147"/>
+      <c r="Y8" s="147"/>
       <c r="Z8" s="90"/>
       <c r="AA8" s="136"/>
       <c r="AB8" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH8" s="137" t="s">
+      <c r="AC8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH8" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI8" s="34"/>
@@ -6632,27 +6656,27 @@
       <c r="AK8" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP8" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ8" s="137" t="s">
+      <c r="AL8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP8" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ8" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR8" s="88"/>
     </row>
-    <row r="9" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="86"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -6683,22 +6707,22 @@
       <c r="AB9" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH9" s="137" t="s">
+      <c r="AC9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH9" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI9" s="34"/>
@@ -6706,27 +6730,27 @@
       <c r="AK9" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP9" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ9" s="137" t="s">
+      <c r="AL9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP9" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ9" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR9" s="88"/>
     </row>
-    <row r="10" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="86"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -6757,22 +6781,22 @@
       <c r="AB10" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH10" s="137" t="s">
+      <c r="AC10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH10" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI10" s="34"/>
@@ -6780,27 +6804,27 @@
       <c r="AK10" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP10" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ10" s="137" t="s">
+      <c r="AL10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP10" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ10" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR10" s="88"/>
     </row>
-    <row r="11" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="86"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -6831,22 +6855,22 @@
       <c r="AB11" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH11" s="137" t="s">
+      <c r="AC11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH11" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI11" s="34"/>
@@ -6854,27 +6878,27 @@
       <c r="AK11" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP11" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ11" s="137" t="s">
+      <c r="AL11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP11" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ11" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR11" s="88"/>
     </row>
-    <row r="12" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="86"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -6905,22 +6929,22 @@
       <c r="AB12" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH12" s="137" t="s">
+      <c r="AC12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH12" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI12" s="34"/>
@@ -6928,27 +6952,27 @@
       <c r="AK12" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP12" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ12" s="137" t="s">
+      <c r="AL12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP12" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ12" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR12" s="88"/>
     </row>
-    <row r="13" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="86"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -6979,22 +7003,22 @@
       <c r="AB13" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH13" s="137" t="s">
+      <c r="AC13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH13" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI13" s="34"/>
@@ -7002,27 +7026,27 @@
       <c r="AK13" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP13" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ13" s="137" t="s">
+      <c r="AL13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP13" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ13" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR13" s="88"/>
     </row>
-    <row r="14" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="86"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -7053,22 +7077,22 @@
       <c r="AB14" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH14" s="137" t="s">
+      <c r="AC14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH14" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI14" s="34"/>
@@ -7076,27 +7100,27 @@
       <c r="AK14" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP14" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ14" s="137" t="s">
+      <c r="AL14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP14" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ14" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR14" s="88"/>
     </row>
-    <row r="15" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="86"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -7127,22 +7151,22 @@
       <c r="AB15" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH15" s="137" t="s">
+      <c r="AC15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH15" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI15" s="34"/>
@@ -7150,27 +7174,27 @@
       <c r="AK15" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP15" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ15" s="137" t="s">
+      <c r="AL15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP15" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ15" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR15" s="88"/>
     </row>
-    <row r="16" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="86"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -7201,22 +7225,22 @@
       <c r="AB16" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH16" s="137" t="s">
+      <c r="AC16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH16" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI16" s="34"/>
@@ -7224,27 +7248,27 @@
       <c r="AK16" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP16" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ16" s="137" t="s">
+      <c r="AL16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP16" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ16" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR16" s="88"/>
     </row>
-    <row r="17" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="86"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -7275,22 +7299,22 @@
       <c r="AB17" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH17" s="137" t="s">
+      <c r="AC17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH17" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI17" s="34"/>
@@ -7298,27 +7322,27 @@
       <c r="AK17" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP17" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ17" s="137" t="s">
+      <c r="AL17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP17" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ17" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR17" s="88"/>
     </row>
-    <row r="18" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="86"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -7347,70 +7371,70 @@
       <c r="Z18" s="75"/>
       <c r="AA18" s="34"/>
       <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
-      <c r="AE18" s="1"/>
-      <c r="AF18" s="1"/>
-      <c r="AG18" s="1"/>
-      <c r="AH18" s="1"/>
+      <c r="AC18" s="140"/>
+      <c r="AD18" s="140"/>
+      <c r="AE18" s="140"/>
+      <c r="AF18" s="140"/>
+      <c r="AG18" s="140"/>
+      <c r="AH18" s="140"/>
       <c r="AI18" s="34"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
-      <c r="AL18" s="1"/>
-      <c r="AM18" s="1"/>
-      <c r="AN18" s="1"/>
-      <c r="AO18" s="1"/>
-      <c r="AP18" s="1"/>
-      <c r="AQ18" s="1"/>
+      <c r="AL18" s="140"/>
+      <c r="AM18" s="140"/>
+      <c r="AN18" s="140"/>
+      <c r="AO18" s="140"/>
+      <c r="AP18" s="140"/>
+      <c r="AQ18" s="140"/>
       <c r="AR18" s="88"/>
     </row>
-    <row r="19" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="86"/>
-      <c r="B19" s="163"/>
-      <c r="C19" s="163"/>
-      <c r="D19" s="163"/>
-      <c r="E19" s="163"/>
+      <c r="B19" s="168"/>
+      <c r="C19" s="168"/>
+      <c r="D19" s="168"/>
+      <c r="E19" s="168"/>
       <c r="F19" s="138"/>
       <c r="G19" s="138"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="167"/>
-      <c r="K19" s="167"/>
-      <c r="L19" s="167"/>
-      <c r="M19" s="167"/>
-      <c r="N19" s="167"/>
-      <c r="O19" s="167"/>
-      <c r="P19" s="167"/>
-      <c r="Q19" s="167"/>
-      <c r="R19" s="167"/>
-      <c r="S19" s="167"/>
-      <c r="T19" s="167"/>
-      <c r="U19" s="167"/>
-      <c r="V19" s="167"/>
-      <c r="W19" s="167"/>
-      <c r="X19" s="167"/>
-      <c r="Y19" s="167"/>
+      <c r="J19" s="172"/>
+      <c r="K19" s="172"/>
+      <c r="L19" s="172"/>
+      <c r="M19" s="172"/>
+      <c r="N19" s="172"/>
+      <c r="O19" s="172"/>
+      <c r="P19" s="172"/>
+      <c r="Q19" s="172"/>
+      <c r="R19" s="172"/>
+      <c r="S19" s="172"/>
+      <c r="T19" s="172"/>
+      <c r="U19" s="172"/>
+      <c r="V19" s="172"/>
+      <c r="W19" s="172"/>
+      <c r="X19" s="172"/>
+      <c r="Y19" s="172"/>
       <c r="Z19" s="25"/>
       <c r="AA19" s="132"/>
       <c r="AB19" s="132"/>
-      <c r="AC19" s="132"/>
-      <c r="AD19" s="132"/>
-      <c r="AE19" s="132"/>
-      <c r="AF19" s="133"/>
-      <c r="AG19" s="74"/>
-      <c r="AH19" s="74"/>
+      <c r="AC19" s="141"/>
+      <c r="AD19" s="141"/>
+      <c r="AE19" s="141"/>
+      <c r="AF19" s="142"/>
+      <c r="AG19" s="141"/>
+      <c r="AH19" s="141"/>
       <c r="AI19" s="34"/>
       <c r="AJ19" s="132"/>
       <c r="AK19" s="132"/>
-      <c r="AL19" s="132"/>
-      <c r="AM19" s="132"/>
-      <c r="AN19" s="132"/>
-      <c r="AO19" s="133"/>
-      <c r="AP19" s="74"/>
-      <c r="AQ19" s="74"/>
+      <c r="AL19" s="141"/>
+      <c r="AM19" s="141"/>
+      <c r="AN19" s="141"/>
+      <c r="AO19" s="142"/>
+      <c r="AP19" s="141"/>
+      <c r="AQ19" s="141"/>
       <c r="AR19" s="88"/>
     </row>
-    <row r="20" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="86"/>
       <c r="B20" s="131" t="s">
         <v>82</v>
@@ -7455,24 +7479,24 @@
       <c r="Z20" s="25"/>
       <c r="AA20" s="134"/>
       <c r="AB20" s="134"/>
-      <c r="AC20" s="134"/>
-      <c r="AD20" s="134"/>
-      <c r="AE20" s="134"/>
-      <c r="AF20" s="165"/>
-      <c r="AG20" s="165"/>
-      <c r="AH20" s="165"/>
+      <c r="AC20" s="143"/>
+      <c r="AD20" s="143"/>
+      <c r="AE20" s="143"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="170"/>
       <c r="AI20" s="34"/>
       <c r="AJ20" s="134"/>
       <c r="AK20" s="134"/>
-      <c r="AL20" s="134"/>
-      <c r="AM20" s="134"/>
-      <c r="AN20" s="134"/>
-      <c r="AO20" s="135"/>
-      <c r="AP20" s="135"/>
-      <c r="AQ20" s="135"/>
+      <c r="AL20" s="143"/>
+      <c r="AM20" s="143"/>
+      <c r="AN20" s="143"/>
+      <c r="AO20" s="144"/>
+      <c r="AP20" s="144"/>
+      <c r="AQ20" s="144"/>
       <c r="AR20" s="88"/>
     </row>
-    <row r="21" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="86"/>
       <c r="B21" s="131" t="s">
         <v>82</v>
@@ -7519,22 +7543,22 @@
       <c r="AB21" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH21" s="137" t="s">
+      <c r="AC21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH21" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI21" s="34"/>
@@ -7542,27 +7566,27 @@
       <c r="AK21" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP21" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ21" s="137" t="s">
+      <c r="AL21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ21" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR21" s="88"/>
     </row>
-    <row r="22" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="86"/>
       <c r="B22" s="131" t="s">
         <v>82</v>
@@ -7609,22 +7633,22 @@
       <c r="AB22" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH22" s="137" t="s">
+      <c r="AC22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH22" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI22" s="34"/>
@@ -7632,27 +7656,27 @@
       <c r="AK22" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP22" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ22" s="137" t="s">
+      <c r="AL22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP22" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ22" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR22" s="88"/>
     </row>
-    <row r="23" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="86"/>
       <c r="B23" s="131" t="s">
         <v>82</v>
@@ -7699,22 +7723,22 @@
       <c r="AB23" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH23" s="137" t="s">
+      <c r="AC23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH23" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI23" s="34"/>
@@ -7722,27 +7746,27 @@
       <c r="AK23" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP23" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ23" s="137" t="s">
+      <c r="AL23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP23" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ23" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR23" s="88"/>
     </row>
-    <row r="24" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="86"/>
       <c r="B24" s="14"/>
       <c r="C24" s="131" t="s">
@@ -7779,22 +7803,22 @@
       <c r="AB24" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH24" s="137" t="s">
+      <c r="AC24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH24" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI24" s="34"/>
@@ -7802,27 +7826,27 @@
       <c r="AK24" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP24" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ24" s="137" t="s">
+      <c r="AL24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP24" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ24" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR24" s="88"/>
     </row>
-    <row r="25" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="86"/>
       <c r="B25" s="14"/>
       <c r="C25" s="131" t="s">
@@ -7842,37 +7866,37 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="166"/>
-      <c r="Q25" s="166"/>
-      <c r="R25" s="166"/>
-      <c r="S25" s="166"/>
-      <c r="T25" s="166"/>
-      <c r="U25" s="166"/>
-      <c r="V25" s="166"/>
-      <c r="W25" s="166"/>
-      <c r="X25" s="166"/>
-      <c r="Y25" s="166"/>
+      <c r="P25" s="171"/>
+      <c r="Q25" s="171"/>
+      <c r="R25" s="171"/>
+      <c r="S25" s="171"/>
+      <c r="T25" s="171"/>
+      <c r="U25" s="171"/>
+      <c r="V25" s="171"/>
+      <c r="W25" s="171"/>
+      <c r="X25" s="171"/>
+      <c r="Y25" s="171"/>
       <c r="Z25" s="12"/>
       <c r="AA25" s="136"/>
       <c r="AB25" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH25" s="137" t="s">
+      <c r="AC25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH25" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI25" s="34"/>
@@ -7880,27 +7904,27 @@
       <c r="AK25" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP25" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ25" s="137" t="s">
+      <c r="AL25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP25" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ25" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR25" s="88"/>
     </row>
-    <row r="26" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="86"/>
       <c r="B26" s="14"/>
       <c r="C26" s="131" t="s">
@@ -7920,37 +7944,37 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="166"/>
-      <c r="Q26" s="166"/>
-      <c r="R26" s="166"/>
-      <c r="S26" s="166"/>
-      <c r="T26" s="166"/>
-      <c r="U26" s="166"/>
-      <c r="V26" s="166"/>
-      <c r="W26" s="166"/>
-      <c r="X26" s="166"/>
-      <c r="Y26" s="166"/>
+      <c r="P26" s="171"/>
+      <c r="Q26" s="171"/>
+      <c r="R26" s="171"/>
+      <c r="S26" s="171"/>
+      <c r="T26" s="171"/>
+      <c r="U26" s="171"/>
+      <c r="V26" s="171"/>
+      <c r="W26" s="171"/>
+      <c r="X26" s="171"/>
+      <c r="Y26" s="171"/>
       <c r="Z26" s="13"/>
       <c r="AA26" s="136"/>
       <c r="AB26" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH26" s="137" t="s">
+      <c r="AC26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH26" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI26" s="34"/>
@@ -7958,27 +7982,27 @@
       <c r="AK26" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP26" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ26" s="137" t="s">
+      <c r="AL26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP26" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ26" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR26" s="88"/>
     </row>
-    <row r="27" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="86"/>
       <c r="B27" s="14"/>
       <c r="C27" s="131" t="s">
@@ -8013,22 +8037,22 @@
       <c r="AB27" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH27" s="137" t="s">
+      <c r="AC27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH27" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI27" s="34"/>
@@ -8036,27 +8060,27 @@
       <c r="AK27" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP27" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ27" s="137" t="s">
+      <c r="AL27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP27" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ27" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR27" s="88"/>
     </row>
-    <row r="28" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="86"/>
       <c r="B28" s="14"/>
       <c r="C28" s="131" t="s">
@@ -8069,11 +8093,11 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="163"/>
-      <c r="L28" s="163"/>
-      <c r="M28" s="163"/>
+      <c r="I28" s="168"/>
+      <c r="J28" s="168"/>
+      <c r="K28" s="168"/>
+      <c r="L28" s="168"/>
+      <c r="M28" s="168"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="24"/>
@@ -8091,22 +8115,22 @@
       <c r="AB28" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH28" s="137" t="s">
+      <c r="AC28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH28" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI28" s="34"/>
@@ -8114,27 +8138,27 @@
       <c r="AK28" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP28" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ28" s="137" t="s">
+      <c r="AL28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP28" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ28" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR28" s="88"/>
     </row>
-    <row r="29" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="86"/>
       <c r="B29" s="6"/>
       <c r="C29" s="131" t="s">
@@ -8179,22 +8203,22 @@
       <c r="AB29" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH29" s="137" t="s">
+      <c r="AC29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH29" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI29" s="34"/>
@@ -8202,27 +8226,27 @@
       <c r="AK29" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP29" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ29" s="137" t="s">
+      <c r="AL29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP29" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ29" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR29" s="88"/>
     </row>
-    <row r="30" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="86"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -8265,22 +8289,22 @@
       <c r="AB30" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH30" s="137" t="s">
+      <c r="AC30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH30" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI30" s="34"/>
@@ -8288,27 +8312,27 @@
       <c r="AK30" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP30" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ30" s="137" t="s">
+      <c r="AL30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP30" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ30" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR30" s="88"/>
     </row>
-    <row r="31" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="86"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -8339,24 +8363,24 @@
       <c r="Z31" s="1"/>
       <c r="AA31" s="34"/>
       <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
-      <c r="AE31" s="1"/>
-      <c r="AF31" s="1"/>
-      <c r="AG31" s="1"/>
-      <c r="AH31" s="1"/>
+      <c r="AC31" s="140"/>
+      <c r="AD31" s="140"/>
+      <c r="AE31" s="140"/>
+      <c r="AF31" s="140"/>
+      <c r="AG31" s="140"/>
+      <c r="AH31" s="140"/>
       <c r="AI31" s="34"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
-      <c r="AL31" s="1"/>
-      <c r="AM31" s="1"/>
-      <c r="AN31" s="1"/>
-      <c r="AO31" s="1"/>
-      <c r="AP31" s="1"/>
-      <c r="AQ31" s="1"/>
+      <c r="AL31" s="140"/>
+      <c r="AM31" s="140"/>
+      <c r="AN31" s="140"/>
+      <c r="AO31" s="140"/>
+      <c r="AP31" s="140"/>
+      <c r="AQ31" s="140"/>
       <c r="AR31" s="88"/>
     </row>
-    <row r="32" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="86"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -8385,24 +8409,24 @@
       <c r="Z32" s="1"/>
       <c r="AA32" s="132"/>
       <c r="AB32" s="132"/>
-      <c r="AC32" s="132"/>
-      <c r="AD32" s="132"/>
-      <c r="AE32" s="132"/>
-      <c r="AF32" s="133"/>
-      <c r="AG32" s="74"/>
-      <c r="AH32" s="74"/>
+      <c r="AC32" s="141"/>
+      <c r="AD32" s="141"/>
+      <c r="AE32" s="141"/>
+      <c r="AF32" s="142"/>
+      <c r="AG32" s="141"/>
+      <c r="AH32" s="141"/>
       <c r="AI32" s="104"/>
       <c r="AJ32" s="132"/>
       <c r="AK32" s="132"/>
-      <c r="AL32" s="132"/>
-      <c r="AM32" s="132"/>
-      <c r="AN32" s="132"/>
-      <c r="AO32" s="133"/>
-      <c r="AP32" s="74"/>
-      <c r="AQ32" s="74"/>
+      <c r="AL32" s="141"/>
+      <c r="AM32" s="141"/>
+      <c r="AN32" s="141"/>
+      <c r="AO32" s="142"/>
+      <c r="AP32" s="141"/>
+      <c r="AQ32" s="141"/>
       <c r="AR32" s="88"/>
     </row>
-    <row r="33" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="86"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -8431,70 +8455,70 @@
       <c r="Z33" s="76"/>
       <c r="AA33" s="134"/>
       <c r="AB33" s="134"/>
-      <c r="AC33" s="134"/>
-      <c r="AD33" s="134"/>
-      <c r="AE33" s="134"/>
-      <c r="AF33" s="135"/>
-      <c r="AG33" s="135"/>
-      <c r="AH33" s="135"/>
+      <c r="AC33" s="143"/>
+      <c r="AD33" s="143"/>
+      <c r="AE33" s="143"/>
+      <c r="AF33" s="144"/>
+      <c r="AG33" s="144"/>
+      <c r="AH33" s="144"/>
       <c r="AI33" s="104"/>
       <c r="AJ33" s="134"/>
       <c r="AK33" s="134"/>
-      <c r="AL33" s="134"/>
-      <c r="AM33" s="134"/>
-      <c r="AN33" s="134"/>
-      <c r="AO33" s="135"/>
-      <c r="AP33" s="135"/>
-      <c r="AQ33" s="135"/>
+      <c r="AL33" s="143"/>
+      <c r="AM33" s="143"/>
+      <c r="AN33" s="143"/>
+      <c r="AO33" s="144"/>
+      <c r="AP33" s="144"/>
+      <c r="AQ33" s="144"/>
       <c r="AR33" s="88"/>
     </row>
-    <row r="34" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="86"/>
       <c r="B34" s="38"/>
-      <c r="C34" s="163"/>
-      <c r="D34" s="163"/>
-      <c r="E34" s="163"/>
-      <c r="F34" s="163"/>
-      <c r="G34" s="163"/>
-      <c r="H34" s="163"/>
-      <c r="I34" s="163"/>
-      <c r="J34" s="163"/>
-      <c r="K34" s="163"/>
-      <c r="L34" s="163"/>
-      <c r="M34" s="163"/>
-      <c r="N34" s="163"/>
-      <c r="O34" s="163"/>
-      <c r="P34" s="163"/>
-      <c r="Q34" s="163"/>
-      <c r="R34" s="163"/>
-      <c r="S34" s="164"/>
-      <c r="T34" s="164"/>
-      <c r="U34" s="164"/>
-      <c r="V34" s="164"/>
-      <c r="W34" s="164"/>
-      <c r="X34" s="164"/>
-      <c r="Y34" s="164"/>
+      <c r="C34" s="168"/>
+      <c r="D34" s="168"/>
+      <c r="E34" s="168"/>
+      <c r="F34" s="168"/>
+      <c r="G34" s="168"/>
+      <c r="H34" s="168"/>
+      <c r="I34" s="168"/>
+      <c r="J34" s="168"/>
+      <c r="K34" s="168"/>
+      <c r="L34" s="168"/>
+      <c r="M34" s="168"/>
+      <c r="N34" s="168"/>
+      <c r="O34" s="168"/>
+      <c r="P34" s="168"/>
+      <c r="Q34" s="168"/>
+      <c r="R34" s="168"/>
+      <c r="S34" s="169"/>
+      <c r="T34" s="169"/>
+      <c r="U34" s="169"/>
+      <c r="V34" s="169"/>
+      <c r="W34" s="169"/>
+      <c r="X34" s="169"/>
+      <c r="Y34" s="169"/>
       <c r="Z34" s="40"/>
       <c r="AA34" s="136"/>
       <c r="AB34" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH34" s="137" t="s">
+      <c r="AC34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH34" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI34" s="34"/>
@@ -8502,45 +8526,45 @@
       <c r="AK34" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP34" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ34" s="137" t="s">
+      <c r="AL34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP34" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ34" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR34" s="88"/>
     </row>
-    <row r="35" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="86"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G35" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H35" s="139" t="s">
+      <c r="C35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I35" s="139" t="s">
@@ -8599,22 +8623,22 @@
       <c r="AB35" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH35" s="137" t="s">
+      <c r="AC35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH35" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI35" s="34"/>
@@ -8622,45 +8646,45 @@
       <c r="AK35" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP35" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ35" s="137" t="s">
+      <c r="AL35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP35" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ35" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR35" s="88"/>
     </row>
-    <row r="36" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="86"/>
       <c r="B36" s="4"/>
-      <c r="C36" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F36" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G36" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H36" s="139" t="s">
+      <c r="C36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H36" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I36" s="139" t="s">
@@ -8719,22 +8743,22 @@
       <c r="AB36" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH36" s="137" t="s">
+      <c r="AC36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH36" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI36" s="34"/>
@@ -8742,45 +8766,45 @@
       <c r="AK36" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP36" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ36" s="137" t="s">
+      <c r="AL36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP36" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ36" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR36" s="88"/>
     </row>
-    <row r="37" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="86"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D37" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F37" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G37" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H37" s="139" t="s">
+      <c r="C37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I37" s="139" t="s">
@@ -8839,22 +8863,22 @@
       <c r="AB37" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH37" s="137" t="s">
+      <c r="AC37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH37" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI37" s="34"/>
@@ -8862,45 +8886,45 @@
       <c r="AK37" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP37" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ37" s="137" t="s">
+      <c r="AL37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP37" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ37" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR37" s="88"/>
     </row>
-    <row r="38" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="86"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F38" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G38" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H38" s="139" t="s">
+      <c r="C38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H38" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I38" s="139" t="s">
@@ -8959,22 +8983,22 @@
       <c r="AB38" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH38" s="137" t="s">
+      <c r="AC38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH38" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI38" s="34"/>
@@ -8982,45 +9006,45 @@
       <c r="AK38" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP38" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ38" s="137" t="s">
+      <c r="AL38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP38" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ38" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR38" s="88"/>
     </row>
-    <row r="39" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="86"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F39" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G39" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H39" s="139" t="s">
+      <c r="C39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H39" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I39" s="139" t="s">
@@ -9079,22 +9103,22 @@
       <c r="AB39" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH39" s="137" t="s">
+      <c r="AC39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH39" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI39" s="34"/>
@@ -9102,45 +9126,45 @@
       <c r="AK39" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP39" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ39" s="137" t="s">
+      <c r="AL39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP39" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ39" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR39" s="88"/>
     </row>
-    <row r="40" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="86"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E40" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F40" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G40" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H40" s="139" t="s">
+      <c r="C40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I40" s="139" t="s">
@@ -9199,22 +9223,22 @@
       <c r="AB40" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH40" s="137" t="s">
+      <c r="AC40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH40" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI40" s="34"/>
@@ -9222,45 +9246,45 @@
       <c r="AK40" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP40" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ40" s="137" t="s">
+      <c r="AL40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP40" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ40" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR40" s="88"/>
     </row>
-    <row r="41" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="86"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F41" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G41" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H41" s="139" t="s">
+      <c r="C41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H41" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I41" s="139" t="s">
@@ -9319,22 +9343,22 @@
       <c r="AB41" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH41" s="137" t="s">
+      <c r="AC41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH41" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI41" s="34"/>
@@ -9342,45 +9366,45 @@
       <c r="AK41" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP41" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ41" s="137" t="s">
+      <c r="AL41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP41" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ41" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR41" s="88"/>
     </row>
-    <row r="42" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="86"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F42" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G42" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H42" s="139" t="s">
+      <c r="C42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H42" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I42" s="139" t="s">
@@ -9439,22 +9463,22 @@
       <c r="AB42" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH42" s="137" t="s">
+      <c r="AC42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH42" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI42" s="34"/>
@@ -9462,45 +9486,45 @@
       <c r="AK42" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP42" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ42" s="137" t="s">
+      <c r="AL42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP42" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ42" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR42" s="88"/>
     </row>
-    <row r="43" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="86"/>
       <c r="B43" s="4"/>
-      <c r="C43" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D43" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E43" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F43" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G43" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H43" s="139" t="s">
+      <c r="C43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H43" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I43" s="139" t="s">
@@ -9559,22 +9583,22 @@
       <c r="AB43" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AC43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH43" s="137" t="s">
+      <c r="AC43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH43" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AI43" s="34"/>
@@ -9582,45 +9606,45 @@
       <c r="AK43" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="AL43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP43" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ43" s="137" t="s">
+      <c r="AL43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP43" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ43" s="131" t="s">
         <v>82</v>
       </c>
       <c r="AR43" s="88"/>
     </row>
-    <row r="44" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="86"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="E44" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F44" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="G44" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="H44" s="139" t="s">
+      <c r="C44" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="H44" s="131" t="s">
         <v>82</v>
       </c>
       <c r="I44" s="139" t="s">
@@ -9694,7 +9718,7 @@
       <c r="AQ44" s="1"/>
       <c r="AR44" s="88"/>
     </row>
-    <row r="45" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:44" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="92"/>
       <c r="B45" s="93"/>
       <c r="C45" s="93"/>
@@ -9759,6 +9783,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="98" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="94" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>